<commit_message>
test with ISP in GeoHashTest first
</commit_message>
<xml_diff>
--- a/LabReport/Lab2/Lab2 (ISP test case design).xlsx
+++ b/LabReport/Lab2/Lab2 (ISP test case design).xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HongDeLiu\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D13560B-69C3-4FC7-BD94-828045FB6D9C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CAEA95B-5FC6-4037-8490-B1F84D0F0AC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="176">
   <si>
     <t>Method</t>
   </si>
@@ -257,6 +258,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>C1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>C1
 C2</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -287,6 +292,798 @@
 T2：{hash="-29jw", expected=-75324}
 T3：{hash="**83", expected=IllegalArgumentException}
 T4：{hash="29jw", expected=75324}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getHashes()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getCharIndex(char ch)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. char ch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return index of the character in characterIndexes map</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1：the character in the characterIndexes map</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1：{True, False}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(T), (F)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1：{ch='b', expected=10}
+T2：{ch='*', expected=IllegalArgumentException}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1 covers {T}
+T2 covers {F}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>padLeftWithZerosToLength(String s, int length)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. String s
+2. int length</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return padded string with left zeros</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NullPointerException</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">C1：s is null
+C2：s.length &gt;= length </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(T, T), (T, F)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(T, T) =&gt; (F, T)
+(T, F) =&gt; (F, F)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1：{s=null, length=8, expected=NullPointerException}
+T2：{s="1234", length=2, expected="1234"}
+T3：{s="1234", length=6, expected="001234"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1 covers {T, T} or {T, F}
+T2 covers {F, T}
+T3 covers {F, F}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CoverageLongs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>build CoverageLongs object first
+1. long[] hashes
+2. int count
+3. double ratio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long[]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return the hashes which are expected to be all of the same length</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1：the relation of hash element number and count
+C2：count (int)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1：{hash element number&lt;count, hash element number=count, hash element number&gt;count}
+C2：{count&lt;0, count=0, count&gt;0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(hash element number&lt;count, count&lt;0), (hash element number&lt;count, count=0), (hash element number&lt;count, count&gt;0)
+, (hash element number=count, count&lt;0), (hash element number=count, count=0), (hash element number=count, count&gt;0)
+, (hash element number&gt;count, count&lt;0), (hash element number&gt;count, count=0), (hash element number&gt;count, count&gt;0)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(hash element number&lt;count, count&lt;0)
+, (hash element number&lt;count, count=0)
+, (hash element number=count, count&lt;0)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(hash element number&lt;count, count&lt;0) =&gt; (hash element number&gt;=0&gt;count, count&lt;0)
+(hash element number&lt;count, count=0) =&gt; (hash element number&gt;=count, couunt=0)
+(hash element number=count, count&lt;0) =&gt; (hash element count&gt;=0&gt;count, count&lt;0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1：{CoverageLongs(hashes={5, 9, 1}, count=5, ratio=1.2), expected=ArrayIndexOutOfBoundsExpection}
+T2：{CoverageLongs(hashes={}, count=0, ratio=1.2), expected={}}
+T3：{CoverageLongs(hashes={5, 9, 1}, count=3, ratio=1.2), expected={5, 9, 1}}
+T4：{CoverageLongs(hashes={5, 9, 1}, count=-3, ratio=1.2), expected=NegativeArraySizeException}
+T5：{CoverageLongs(hashes={5, 9, 1}, count=0, ratio=1.2), expected={}}
+T6：{CoverageLongs(hashes={5, 9, 1}, count=2, ratio=1.2), expected={5, 9}}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1 covers {hash element number&lt;count, count&gt;0}
+T2 covers {hash element number=count, count=0}
+T3 covers {hash element number=count, count&gt;0}
+T4 covers {hash element number&gt;count, count&lt;0}
+T5 covers {hash element number&gt;count, count=0}
+T6 covers {hash element number&gt;count, count&gt;0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ArrayIndexOutOfBoundsExpection
+NegativeArraySizeException</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getRatio()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>double</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return ratio of area of hashes to area of target region</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1：ratio (double)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1：{ratio&lt;0, ratio=0, ratio&gt;0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(ratio&lt;0), (ratio=0), (ratio&gt;0)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1：{CoverageLongs(hashes={5, 9, 1}, count=3, ratio=-1.2), expected=-1.2}
+T2：{CoverageLongs(hashes={5, 9, 1}, count=3, ratio=0), expected=0}
+T3：{CoverageLongs(hashes={5, 9, 1}, count=3, ratio=1.2), expected=1.2}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1 covers {ratio&lt;0}
+T2 covers {ratio=0}
+T3 covers {ratio&gt;0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n/a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getHashLength()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return the length in characters of the first hash returned by an iterator on the hash set.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1：{hashes[0]&lt;=-16, -16&lt;has[0]hes&lt;16, hashes[0]&gt;=16}
+C2：{count&lt;0, count=0, count&gt;0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(hashes[0]&lt;=-16, count&lt;0), (hashes[0]&lt;=-16, count=0), (hashes[0]&lt;=-16, count&gt;0)
+, (-16&lt;hashes[0]&lt;16, count&lt;0), (-16&lt;hashes[0]&lt;16, count=0), (-16&lt;hashes[0]&lt;16, count&gt;0)
+, (hashes[0]&gt;=16, count&lt;0), (hashes[0]&gt;=16, count=0), (hashes[0]&gt;=16, count&gt;0)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1 covers {hashes[0]&lt;=-16, count&lt;0}
+T2 covers {hashes[0]&lt;=-16, count=0}
+T3 covers {hashes[0]&lt;=-16, count&gt;0}
+T4 covers {-16&lt;hashes[0]&lt;16, count&lt;0}
+T5 covers {-16&lt;hashes[0]&lt;16, count=0}
+T6 covers {-16&lt;hashes[0]&lt;16, count=0}
+T7 covers {hashes[0]&gt;=16, count&lt;0}
+T8 covers {hashes[0]&gt;=16, count=0}
+T9 covers {hashes[0]&gt;=16, count&gt;0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1：the first element hash set number logical and with 1111
+C2：count (int)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1：{CoverageLongs(hashes={-20, 9, 1}, count=-1, ratio=1.2), expected=12}
+T2：{CoverageLongs(hashes={-20, 9, 1}, count=0, ratio=1.2), expected=0}
+T3：{CoverageLongs(hashes={-20, 9, 1}, count=1, ratio=1.2), expected=12}
+T4：{CoverageLongs(hashes={5, 9, 1}, count=-1, ratio=1.2), expected=5}
+T5：{CoverageLongs(hashes={5, 9, 1}, count=0, ratio=1.2), expected=0}
+T6：{CoverageLongs(hashes={5, 9, 1}, count=1, ratio=1.2), expected=5}
+T7：{CoverageLongs(hashes={20, 9, 1}, count=-1, ratio=1.2), expected=4}
+T8：{CoverageLongs(hashes={20, 9, 1}, count=0, ratio=1.2), expected=0}
+T9：{CoverageLongs(hashes={20, 9, 1}, count=1, ratio=1.2), expected=4}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1
+C2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getCount()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return the count</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1：count (int)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1：{count&lt;0, count=0, count&gt;0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(count&lt;0), (count=0), (count&gt;0)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">T1：{CoverageLongs(hashes={5, 9, 1}, count=-1, ratio=1.2), expected=-1}
+T2：{CoverageLongs(hashes={5, 9, 1}, count=0, ratio=1.2), expected=0}
+T3：{CoverageLongs(hashes={5, 9, 1}, count=1, ratio=1.2), expected=1} </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1 covers {count&lt;0}
+T2 covers {count=0}
+T3 covers {count&gt;0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GeoHash</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adjacentHash(String hash, Direction direction)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. String hash
+2. Direction direction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return the adjacent hash in given</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1：hash is null
+C2：hash.length &gt; 0
+C3：direction (Direction)
+C4：hash in border</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1：{True, False}
+C2：{True, False}
+C3：{top, bottom, left, right}
+C4：{True, False}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(T, T, top, T), (T, T, bottom, T), (T, T, left, T), (T, T, right, T), (T, T, top, F), (T, T, bottom, F), (T, T, left, F), (T, T, right, F)
+, (T, F, top, T), (T, F, bottom, T), (T, F, left, T), (T, F, right, T), (T, F, top, F), (T, F, bottom, F), (T, F, left, F), (T, F, right, F)
+, (F, T, top, T), (F, T, bottom, T), (F, T, left, T), (F, T, right, T), (F, T, top, F), (F, T, bottom, F), (F, T, left, F), (F, T, right, F)
+, (F, F, top, T), (F, F, bottom, T), (F, F, left, T), (F, F, right, T), (F, F, top, F), (F, F, bottom, F), (F, F, left, F), (F, F, right, F)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(T, T, direction, T), (T, T, direction, F)
+, (T, F, direction, T), (T, F, direction, F)
+, (F, F, direction, T), (F, F, direction, F)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1 covers {T, T(F), direction, T(F)}
+T2 covers {F, T, top, T}
+T3 covers {F, T, bottom, T}
+T4 covers {F, T, left, T}
+T5 covers {F, T, right, T}
+T6 covers {F, T, top, F}
+T7 covers {F, T, bottom, F}
+T8 covers {F, T, left, F}
+T9 covers {F, T, right, F}
+T10 covers {F, F, direction T(F)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>right(String hash)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. String hash</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">return the adjacent hash to the right (east) </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1
+C2
+C3
+C4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1：hash is null
+C2：hash.length &gt; 0
+C3：hash in border</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1：{True, False}
+C2：{True, False}
+C3：{True, False}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(T, T, T), (T, T, F), (T, F, T), (T, F, F)
+, (F, T, T), (F, T, F), (F, F, T), (F, F, F)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(T, T, T), (T, T, F), (T, F, T), (T, F, F)
+, (F, F, T), (F, F, F)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1：{hashes=null, direction=top, expected=IllegalArgumentException}
+T2：{hashes="dx", direction=top, expected="f8"}
+T3：{hashes="d2", direction=bottom, expected="6r"}
+T4：{hashes="d4", direction=left, expected="9f"}
+T5：{hashes="dg", direction=right, expected="e5"}
+T6：{hashes="k", direction=top, expected="s"}
+T7：{hashes="k", direction=bottom, expected="h"}
+T8：{hashes="k", direction=left, expected="7"}
+T9：{hashes="k", direction=right, expected="m"}
+T10：{hashes="", direction=top, expected=IllegalArgumentException}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1：{hashes=null, expected=IllegalArgumentException}
+T2：{hashes="dg", expected="e5"}
+T3：{hashes="k", expected="m"}
+T4：{hashes="", expected=IllegalArgumentException}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1 covers {T, T(F), T(F)}
+T2 covers {F, T, T}
+T3 covers {F, T, F}
+T4 covers {F, F, T(F)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>left(String hash)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">return the adjacent hash to the left (west) </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1
+C2
+C3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1：{hashes=null, expected=IllegalArgumentException}
+T2：{hashes="d4", expected="9f"}
+T3：{hashes="k", expected="7"}
+T4：{hashes="", expected=IllegalArgumentException}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>top(String hash)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">return the adjacent hash to the top (north) </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1：{hashes=null, expected=IllegalArgumentException}
+T2：{hashes="dx", expected="f8"}
+T3：{hashes="k", expected="s"}
+T4：{hashes="", expected=IllegalArgumentException}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bottom(String hash)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">return the adjacent hash to the bottom (south) </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1：{hashes=null, expected=IllegalArgumentException}
+T2：{hashes="d2", expected="6r"}
+T3：{hashes="k", expected="h"}
+T4：{hashes="", expected=IllegalArgumentException}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adjacentHash(String hash, Direction direction, int steps)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. String hash
+2. Direction direction
+3. int steps</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return the adjacent hash N steps in the given.
+A negative N will use the opposite</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1：hash is null
+C2：hash.length &gt; 0
+C3：direction (Direction)
+C4：hash in border
+C5：steps (int)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1：{True, False}
+C2：{True, False}
+C3：{top, bottom, left, right}
+C4：{True, False}
+C5：{steps&lt;0, steps=0, steps&gt;0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(T, T, top, T, steps&lt;0), (T, T, bottom, T, steps&lt;0), (T, T, left, T, steps&lt;0), (T, T, right, T, steps&lt;0), (T, T, top, F, steps&lt;0), (T, T, bottom, F, steps&lt;0), (T, T, left, F, steps&lt;0), (T, T, right, F, steps&lt;0)
+, (T, T, top, T, steps=0), (T, T, bottom, T, steps=0), (T, T, left, T, steps=0), (T, T, right, T, steps=0), (T, T, top, F, steps=0), (T, T, bottom, F, steps=0), (T, T, left, F, steps=0), (T, T, right, F, steps=0)
+, (T, T, top, T, steps&gt;0), (T, T, bottom, T, steps&gt;0), (T, T, left, T, steps&gt;0), (T, T, right, T, steps&gt;0), (T, T, top, F, steps&gt;0), (T, T, bottom, F, steps&gt;0), (T, T, left, F, steps&gt;0), (T, T, right, F, steps&gt;0)
+, (T, F, top, T, steps&lt;0), (T, F, bottom, T, steps&lt;0), (T, F, left, T, steps&lt;0), (T, F, right, T, steps&lt;0), (T, F, top, F, steps&lt;0), (T, F, bottom, F, steps&lt;0), (T, F, left, F, steps&lt;0), (T, F, right, F, steps&lt;0)
+, (T, F, top, T, steps=0), (T, F, bottom, T, steps=0), (T, F, left, T, steps=0), (T, F, right, T, steps=0), (T, F, top, F, steps=0), (T, F, bottom, F, steps=0), (T, F, left, F, steps=0), (T, F, right, F, steps=0)
+, (T, F, top, T, steps&gt;0), (T, F, bottom, T, steps&gt;0), (T, F, left, T, steps&gt;0), (T, F, right, T, steps&gt;0), (T, F, top, F, steps&gt;0), (T, F, bottom, F, steps&gt;0), (T, F, left, F, steps&gt;0), (T, F, right, F, steps&gt;0)
+, (F, T, top, T, steps&lt;0), (F, T, bottom, T, steps&lt;0), (F, T, left, T, steps&lt;0), (F, T, right, T, steps&lt;0), (F, T, top, F, steps&lt;0), (F, T, bottom, F, steps&lt;0), (F, T, left, F, steps&lt;0), (F, T, right, F, steps&lt;0)
+, (F, T, top, T, steps=0), (F, T, bottom, T, steps=0), (F, T, left, T, steps=0), (F, T, right, T, steps=0), (F, T, top, F, steps=0), (F, T, bottom, F, steps=0), (F, T, left, F, steps=0), (F, T, right, F, steps=0)
+, (F, T, top, T, steps&gt;0), (F, T, bottom, T, steps&gt;0), (F, T, left, T, steps&gt;0), (F, T, right, T, steps&gt;0), (F, T, top, F, steps&gt;0), (F, T, bottom, F, steps&gt;0), (F, T, left, F, steps&gt;0), (F, T, right, F, steps&gt;0)
+, (F, F, top, T, steps&lt;0), (F, F, bottom, T, steps&lt;0), (F, F, left, T, steps&lt;0), (F, F, right, T, steps&lt;0), (F, F, top, F, steps&lt;0), (F, F, bottom, F, steps&lt;0), (F, F, left, F, steps&lt;0), (F, F, right, F, steps&lt;0)
+, (F, F, top, T, steps=0), (F, F, bottom, T, steps=0), (F, F, left, T, steps=0), (F, F, right, T, steps=0), (F, F, top, F, steps=0), (F, F, bottom, F, steps=0), (F, F, left, F, steps=0), (F, F, right, F, steps=0)
+, (F, F, top, T, steps&gt;0), (F, F, bottom, T, steps&gt;0), (F, F, left, T, steps&gt;0), (F, F, right, T, steps&gt;0), (F, F, top, F, steps&gt;0), (F, F, bottom, F, steps&gt;0), (F, F, left, F, steps&gt;0), (F, F, right, F, steps&gt;0)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(T, T(F), direction, T(F),steps) =&gt; (F, T(F), direction, T(F), steps)
+(F, F, direction, T(F), steps) =&gt; (F, T, direction, T(F), steps)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(T, T, direction, T) =&gt; (F, T, direction, T)
+(T, T, direction, F) =&gt; (F, T, direction, F)
+(T, F, direction, T) =&gt; (F, F, direction, T)
+(T, F, direction, F) =&gt; (F, F, direction, F)
+(F, F, direction, T) =&gt; (F, T, direction, T)
+(F, F, direction, F) =&gt; (F, T, direction, F)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(T, T, T) =&gt; (F, T, T)
+(T, T, F) =&gt; (F, T, F)
+(T, F, T) =&gt; (F, F, T)
+(T, F, F) =&gt; (F, F, F)
+(F, F, T) =&gt; (F, T, T)
+(F, F, F) =&gt; (F, T, F)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1
+C2
+C3
+C4
+C5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(T, T(F), direction, T(F), steps(&gt;0 or &lt;0)), (F, F, direction, T(F), steps)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1：{hashes=null, direction=top, steps=2, expected=IllegalArgumentException}
+T2：{hashes=null, direction=right, steps=0, expected=null}
+T3：{hashes="d2", direction=top, steps=-2, expected="6q"}
+T4：{hashes="d2", direction=top, step=0, expected="d2"}
+T5：{hashes="dx", direction=top, step=2, expected="f9"}
+T6：{hashes="dx", direction=bottom, steps=-2, expected="f9"}
+T7：{hashes="dx", direction=bottom, steps=0, expected="dx"}
+T8：{hashes="d2", direction=bottom, steps=2, expected="6q"}
+T9：{hashes="dg", direction=left, steps=-2, expected="e7"}
+T10：{hashes="dg", direction=left, steps=0, expected="dg"}
+T11：{hashes="d4", direction=left, steps=2, expected="9d"}
+T12：{hashes="d4", direction=right, steps=-2, expected="9d"}
+T13：{hashes="d4", direction=right, steps=0, expected="d4"}
+T14：{hashes="dg", direction=right, steps=2, expected="e7"}
+T15：{hashes="7k", direction=top, steps=-2, expected="76"}
+T16：{hashes="7k", direction=top, steps=0, expected="7k"}
+T17：{hashes="7k", direction=top, steps=2, expected="7q"}
+T18：{hashes="7k", direction=bottom, steps=-2, expected="7q"}
+T19：{hashes="7k", direction=bottom, steps=0, expected="7k"}
+T20：{hashes="7k", direction=bottom, steps=2, expected="76"}
+T21：{hashes="7k", direction=left, steps=-2, expected="7u"}
+T22：{hashes="7k", direction=left, steps=0, expected="7k"}
+T23：{hashes="7k", direction=left, steps=2, expected="6u"}
+T24：{hashes="7k", direction=right, steps=-2, expected="6u"}
+T25：{hashes="7k", direction=right, steps=0, expected="7k"}
+T26：{hashes="7k", direction=right, steps=2, expected="7u"}
+T27：{hashes="", direction=top, steps=2, expected=IllegalArgumentException}
+T28：{hashes="", direction=right, steps=0, expected=""}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1 covers {T, T(F), direction, T(F), steps(&gt;0 or &lt;0)}
+T2 covers {T, T(F), direction, T(F), steps=0}
+T3 covers {F, T, top, T, steps&lt;0}
+T4 covers {F, T, top, T, steps=0}
+T5 covers {F, T, top, T, steps&gt;0}
+T6 covers {F, T, bottom, T, steps&lt;0}
+T7 covers {F, T, bottom, T, steps=0}
+T8 covers {F, T, bottom, T, steps&gt;0}
+T9 covers {F, T, left, T, steps&lt;0}
+T10 covers {F, T, left, T, steps=0}
+T11 covers {F, T, left, T, steps&gt;0}
+T12 covers {F, T, right, T, steps&lt;0}
+T13 covers {F, T, right, T, steps=0}
+T14 covers {F, T, right, T, steps&gt;0}
+T15 covers {F, T, top, F, steps&lt;0}
+T16 covers {F, T, top, F, steps=0}
+T17 covers {F, T, top, F, steps&gt;0}
+T18 covers {F, T, bottom, F, steps&lt;0}
+T19 covers {F, T, bottom, F, steps=0}
+T20 covers {F, T, bottom, F, steps&gt;0}
+T21 covers {F, T, left, F, steps&lt;0}
+T22 covers {F, T, left, F, steps=0}
+T23 covers {F, T, left, F, steps&gt;0}
+T24 covers {F, T, right, F, steps&lt;0}
+T25 covers {F, T, right, F, steps=0}
+T26 covers {F, T, right, F, steps&gt;0}
+T27 covers {F, F, direction, T(F), steps(&gt;0 or &lt;0)}
+T28 covers {F, F, direction, T(F), steps=0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nrighbours(String hash)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>List&lt;String&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return a list of the 8 surrounding hashes for a given hash in order left, right, top, bottom, left-top, left-bottom, right-top, right-bottom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1：hash is null
+C2：hash.length&gt;0
+C3：hash in border</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1：{hashes=null, expected=IllegalArgumentException}
+T2：{hashes="d2", expected=&lt;"d0", "d8", "d3", "6r", "d1", "6p","d9", "6x"&gt;}
+T3：{hashes="k", expected=&lt;"7", "m", "s", "h", "e", "5", "t", "j"&gt;}
+T4：{hashes="", expected=IllegalArgumentException}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>encodeHash(double latitude, double longitude)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. double latitude
+2. double longitude</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1：latitude (double)
+C2：longitude (double)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1：{latitude&lt;-90, -90&lt;=latitude&lt;=90, latiyud&gt;90}
+C2：{longitude&lt;-180, -180&lt;=longitude&lt;=180, longitude&gt;180}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(latitude&lt;-90, longitude&lt;-180), (latitude&lt;-90, -180&lt;=longitude&lt;=180), (latitude&lt;-90, longitude&gt;180)
+, (-90&lt;=latitude&lt;=90, longitude&lt;-180), (-90&lt;=latitude&lt;=90, -180&lt;=longitude&lt;=180), (-90&lt;=latitude&lt;=90, longitude&gt;180)
+, (latitude&gt;90, longitude&lt;-180), (latitude&gt;90, -180&lt;=longitude&lt;180), (latitude&gt;90, longitude&gt;180)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1：{latitude=-100, longitude=-200, expected=IllegalArgumentException}
+T2：{latitude=-100, longitude=50, expected=IllegalArgumentException}
+T3：{latitude=-100, longitude=200, expected=IllegalArgumentException}
+T4：{latiturde=50, longitude=-200, expected="z8cu2yhrn5x1"}
+T5：{latitude=50, longitude=50, expected="v0gs3y0zh7w1"}
+T6：{latitude=50, longitude=200, expected="b2yhrn5x1g8c"}
+T7：{latitude=100, longitude=-200, expected=IllegalArgumentExpection}
+T8：{latitude=100, longitude=50, expected=IllegalArgumentException}
+T9：{latitude=100, longitude=200, expected=IllegalArgumentException}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1 covers {latitude&lt;-90, longitude&lt;-180}
+T2 covers {latitude&lt;-90, -180&lt;=longitude&lt;=180}
+T3 covers {latitude&lt;-90, longitude&gt;180}
+T4 covers {-90&lt;=latitude&lt;=90, longitude&lt;-180}
+T5 covers {-90&lt;=latitude&lt;=90, -180&lt;=longitude&lt;=180}
+T6 covers {-90&lt;=latitude&lt;=90, longitude&gt;180}
+T7 covers {latitude&gt;90, longitude&lt;-180}
+T8 covers {latitude&gt;90, -180&lt;=longitude&lt;=180}
+T9 covers {latitude&gt;90, longitude&gt;180}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>encodeHash(LatLong p, int length)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>build LatLong object first
+1. double lat
+2. double lon
+3, int length</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return  a geoHash of given length for the giver latitude and longitude</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return a geohash of length 12 for the given latitude and longitude</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1：latitude (double)
+C2：longitude (double)
+C3：length (int)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1：{latitude&lt;-90, -90&lt;=latitude&lt;=90, latiyud&gt;90}
+C2：{longitude&lt;-180, -180&lt;=longitude&lt;=180, longitude&gt;180}
+C3：{length&lt;=0, 0&lt;length&lt;=12, length&gt;12}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(LatLong(lat&lt;-90, lon&lt;-180), length&lt;=0), (LatLong(lat&lt;-90, lon&lt;-180), 0&lt;length&lt;=12), (LatLong(lat&lt;-90, lon&lt;-180), length&gt;12)
+, (LatLong(lat&lt;-90, -180&lt;=lon&lt;=180), length&lt;=0), (LatLong(lat&lt;-90, -180&lt;=lon&lt;=180), 0&lt;length&lt;=12), (LatLong(lat&lt;-90, -180&lt;=lon&lt;=180),length&gt;12)
+, (LatLong(lat&lt;-90, lon&gt;180), length&lt;=0), (LatLong(lat&lt;-90, lon&gt;180), 0&lt;length&lt;=12), (LatLong(lat&lt;-90, lon&gt;180), length&gt;12)
+, (LatLong(-90&lt;=lat&lt;=90, lon&lt;-180), length&lt;=0), (LatLong(-90&lt;=lat&lt;=90, lon&lt;-180), 0&lt;length&lt;=12), (LatLong(-90&lt;=lat&lt;=90, lon&lt;-180), length&gt;12)
+, (LatLong(-90&lt;=lat&lt;=90, -180&lt;=lon&lt;=180), length&lt;=0), (LatLong(-90&lt;=lat&lt;=90, -180&lt;=lon&lt;=180), 0&lt;length&lt;=12), (LatLong(-90&lt;=lat&lt;=90, -180&lt;=lon&lt;=180), length&gt;12)
+, (LatLong(-90&lt;=lat&lt;=90, lon&gt;180), length&lt;=0), (LatLong(-90&lt;=lat&lt;=90, lon&gt;180), 0&lt;length&lt;=12), (LatLong(-90&lt;=lat&lt;=90,lon&gt;180), length&gt;12)
+, (LatLong(lat&gt;90, lon&lt;-180), length&lt;=0), (LatLong(lat&gt;90, lon&lt;-180), 0&lt;length&lt;=12), (LatLong(lat&gt;90, lon&lt;-180), length&gt;12)
+, (LatLong(lat&gt;90, -180&lt;=lon&lt;=180), length&lt;=0), (LatLong(lat&gt;90, -180&lt;=lon&lt;=180), 0&lt;length&lt;=12), (LatLong(lat&gt;90, -180&lt;=lon&lt;=180), length&gt;12)
+, (LatLong(lat&gt;90, lon&gt;180), length&lt;=0), (LatLong(lat&gt;90, lon&gt;180), 0&lt;length&lt;=12), (LatLong(lat&gt;90, lon&gt;180), length&gt;12)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1：{LatLong(lat=-100, lon=50), length=12, expeceted=IllegalArgumentException}
+T2：{LatLong(lat=50, lon=-200), length=0, expected=IllegalArgumentException}
+T3：{LatLong(lat=50, lon=-200), length=12, expected="z8cu2yhrn5x1"}
+T4：{LatLong(lat=50, lon=-200), length=13, expected=IllegalArgumentException}
+T5：{LatLong(lat=50, lon=50), length=12, expected="v0gs3y0zh7w1"}
+T6：{LatLong(lat=50, lon=200), length=12, expected-"b2yhrn5x1g8c"}
+T7：{LatLong(lat=100, lon=50), length=12, expected=IllegalArgumentException}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1 covers {LatLong(lat&lt;-90, lon), length}
+T2 covers {LatLong(lat, lon), length&lt;=0}
+T3 covers {LatLong(-90&lt;=lat&lt;=90, lon&lt;-180), 0&lt;length&lt;=12}
+T4 covers {LatLong(lat, lon), length&gt;12}
+T5 covers {LatLong(-90&lt;=lat&lt;=90, -180&lt;=lon&lt;=180), 0&lt;length&lt;=12}
+T6 covers {LatLong(-90&lt;=lat&lt;=90, lon&gt;180), 0&lt;length&lt;=12}
+T7 covers {LatLong(lat&gt;90, lon), length}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>encodeHash(LatLong p)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>build LatLong object first
+1. double lat
+2. double lon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return  a geoHash of length 12 for the giver latitude and longitude</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(LatLong(lat&lt;-90, lon&lt;-180)), (LatLong(lat&lt;-90, -180&lt;=lon&lt;=180)), (LatLong(lat&lt;-90, lon&gt;180))
+, (LatLong(-90&lt;=lat&lt;=90, lon&lt;-180)), (LatLong(-90&lt;=lat&lt;=90, -180&lt;=lon&lt;=180)), (LatLong(-90&lt;=lat&lt;=90, lon&gt;180))
+, (LatLong(lat&gt;90, lon&lt;-180)), (LatLong(lat&gt;90, -180&lt;=lon&lt;=180)), (LatLong(lat&gt;90, lon&gt;180))}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1：{LatLong(lat=-100, lon=-200), expected=IllegalArgumentException}
+T2：{LatLong(lat=-100, lon=50), expected=IllegalArgumentException}
+T3：{LatLong(lat=-100, lon=200), expected=IllegalArgumentException}
+T4：{LatLong(lat=50, lon=-200), expected="z8cu2yhrn5x1"}
+T5：{LatLong(lat=50, lon=50), expected="v0gs3y0zh7w1"}
+T6：{LatLong(lat=50, lon=200), expected="b2yhrn5x1g8c"}
+T7：{LatLong(lat=100, lon=-200), expected=IllegalArgumentException}
+T8：{LatLong(lat=100, lon=50), expected=IllegalArgumentException}
+T9：{LatLong(lat=100, lon=200), expected=IllegalArgumentExpection}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1 covers {LatLong(lat&lt;-90, lon&lt;-180)}
+T2 covers {LatLong(lat&lt;-90, -180&lt;=lon&lt;=180)}
+T3 covers {LatLong(lat&lt;-90, lon&gt;180)}
+T4 covers {LatLong(-90&lt;=lat&lt;=90, lon&lt;-180)}
+T5 covers {LatLong(-90&lt;=lat&lt;=90, -180&lt;=lon&lt;=180)}
+T6 covers {LatLong(-90&lt;=lat&lt;=90, lon&gt;180)}
+T7 covers {LatLong(lat&gt;90, lon&lt;-180)}
+T8 covers {LatLong(lat&gt;90, -180&lt;=lon&lt;180)}
+T9 covers {LatLong(lat&gt;90, lon&gt;180)}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -294,6 +1091,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -356,7 +1156,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -367,6 +1167,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -649,31 +1455,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="M18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" customWidth="1"/>
-    <col min="5" max="5" width="86.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5546875" customWidth="1"/>
+    <col min="1" max="1" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="115" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.5" customWidth="1"/>
+    <col min="7" max="7" width="16.5" customWidth="1"/>
     <col min="8" max="8" width="65" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="34.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="55.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.44140625" customWidth="1"/>
-    <col min="12" max="12" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="50.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="71.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="157.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.25" customWidth="1"/>
+    <col min="12" max="12" width="65.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="84.75" customWidth="1"/>
+    <col min="14" max="14" width="54.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -717,8 +1523,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="145.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:14" ht="148.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
@@ -761,10 +1567,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="48.6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
+    <row r="3" spans="1:14" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
       <c r="B3" t="s">
         <v>28</v>
       </c>
@@ -805,10 +1609,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="64.8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
+    <row r="4" spans="1:14" ht="66" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
       <c r="B4" t="s">
         <v>36</v>
       </c>
@@ -825,16 +1627,16 @@
         <v>40</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>22</v>
@@ -843,16 +1645,711 @@
         <v>22</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N4" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="33" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>44</v>
       </c>
+      <c r="K6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="M5" s="2"/>
+    <row r="7" spans="1:14" ht="115.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="66" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="148.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="66" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E10" t="s">
+        <v>99</v>
+      </c>
+      <c r="F10" t="s">
+        <v>88</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="184.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E11" t="s">
+        <v>109</v>
+      </c>
+      <c r="F11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="99" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D12" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12" t="s">
+        <v>117</v>
+      </c>
+      <c r="F12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="99" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" t="s">
+        <v>127</v>
+      </c>
+      <c r="F13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="99" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" t="s">
+        <v>130</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D14" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" t="s">
+        <v>131</v>
+      </c>
+      <c r="F14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="99" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" t="s">
+        <v>133</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D15" t="s">
+        <v>108</v>
+      </c>
+      <c r="E15" t="s">
+        <v>134</v>
+      </c>
+      <c r="F15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" t="s">
+        <v>136</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D16" t="s">
+        <v>108</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="99" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" t="s">
+        <v>149</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" t="s">
+        <v>150</v>
+      </c>
+      <c r="E17" t="s">
+        <v>151</v>
+      </c>
+      <c r="F17" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="165" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B18" t="s">
+        <v>154</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" t="s">
+        <v>164</v>
+      </c>
+      <c r="F18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="148.5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" t="s">
+        <v>161</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" t="s">
+        <v>163</v>
+      </c>
+      <c r="F19" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="148.5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>105</v>
+      </c>
+      <c r="B20" t="s">
+        <v>170</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" t="s">
+        <v>172</v>
+      </c>
+      <c r="F20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>175</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A10"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>